<commit_message>
628805: TASK: Requirements Traceability Matrix for IOC Entry TASCore Build 3 in Requirement Folder - Revised to be consistent with RTM
</commit_message>
<xml_diff>
--- a/TASCore_documents/Requirement/Build 3/TAS_Core_RTM_TAS.01.00.203_20180607_163807.xlsx
+++ b/TASCore_documents/Requirement/Build 3/TAS_Core_RTM_TAS.01.00.203_20180607_163807.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\TASCore\Build 3\Release Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.ballerstein\Desktop\latest\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042B6D99-D8AB-4BDF-8FE7-A2D0800384F7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="RTM" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RTM!$A$1:$J$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RTM!$A$1:$J$75</definedName>
     <definedName name="OutSharedNoteLink" localSheetId="2">RTM!$A$24</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="130">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -427,8 +428,23 @@
     </r>
   </si>
   <si>
+    <t>Comments Failed US- Defect ID Not Testable Comment</t>
+  </si>
+  <si>
+    <t>June 18, 2018</t>
+  </si>
+  <si>
+    <t>DE482</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>July 17, 2018</t>
+  </si>
+  <si>
     <r>
-      <t>Version 2.0</t>
+      <t>Version 3.0</t>
     </r>
     <r>
       <rPr>
@@ -442,138 +458,21 @@
     </r>
   </si>
   <si>
-    <t>US3581</t>
-  </si>
-  <si>
-    <t>Review New v2.0 508 compliance user stories</t>
-  </si>
-  <si>
-    <t>TC2817</t>
-  </si>
-  <si>
-    <t>TC2818</t>
-  </si>
-  <si>
-    <t>TC2819</t>
-  </si>
-  <si>
-    <t>DE644</t>
-  </si>
-  <si>
-    <t>DE645</t>
-  </si>
-  <si>
-    <t>DE646</t>
-  </si>
-  <si>
-    <t>DE643</t>
-  </si>
-  <si>
-    <t>DE647</t>
-  </si>
-  <si>
-    <t>DE648</t>
-  </si>
-  <si>
-    <t>TC2822</t>
-  </si>
-  <si>
-    <t>DE649</t>
-  </si>
-  <si>
-    <t>TC2823</t>
-  </si>
-  <si>
-    <t>DE650</t>
-  </si>
-  <si>
-    <t>DE651</t>
-  </si>
-  <si>
-    <t>TC2824</t>
-  </si>
-  <si>
-    <t>DE652</t>
-  </si>
-  <si>
-    <t>DE733</t>
-  </si>
-  <si>
-    <t>Comments Failed US- Defect ID Not Testable Comment</t>
-  </si>
-  <si>
-    <t>DE723</t>
-  </si>
-  <si>
-    <t>DE725</t>
-  </si>
-  <si>
-    <t>DE729</t>
-  </si>
-  <si>
-    <t>DE732</t>
-  </si>
-  <si>
-    <t>DE766</t>
-  </si>
-  <si>
-    <t>TC1492</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Define Layout of the MCCF EDI Home Page</t>
-  </si>
-  <si>
-    <t>TC1561</t>
-  </si>
-  <si>
-    <t>TC2820</t>
-  </si>
-  <si>
-    <t>June 18, 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review New v2.0 508 compliance user stories </t>
-  </si>
-  <si>
-    <t>TC2143</t>
-  </si>
-  <si>
-    <t>TC3366</t>
-  </si>
-  <si>
-    <t>TC3367</t>
-  </si>
-  <si>
-    <t>TC3368</t>
-  </si>
-  <si>
-    <t>DE482</t>
-  </si>
-  <si>
-    <t>DE720, DE552</t>
-  </si>
-  <si>
-    <t>TC1180</t>
-  </si>
-  <si>
-    <t>DE553</t>
-  </si>
-  <si>
-    <t>TC1186</t>
-  </si>
-  <si>
-    <t>DE554, DE555</t>
+    <t>was impacted by DE485 (discovered in TC2177)</t>
+  </si>
+  <si>
+    <t>was impacted by DE518 (discovered in TC2362)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -788,6 +687,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1272,7 +1175,7 @@
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1336,16 +1239,25 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1402,7 +1314,7 @@
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
@@ -1680,12 +1592,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Revision_History" displayName="Revision_History" ref="A3:D5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Revision_History" displayName="Revision_History" ref="A3:D6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" name="Version" dataDxfId="2"/>
-    <tableColumn id="3" name="Description" dataDxfId="1"/>
-    <tableColumn id="4" name="Author" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Version" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Author" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2011,137 +1923,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection activeCell="A20" sqref="A20:H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="21.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-    </row>
-    <row r="7" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-    </row>
-    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
     </row>
   </sheetData>
@@ -2159,34 +2071,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="19.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-    </row>
-    <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -2200,7 +2112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
@@ -2214,9 +2126,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="B5" s="18">
         <v>2</v>
@@ -2228,49 +2140,60 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="18">
+        <v>3</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
     </row>
   </sheetData>
@@ -2286,34 +2209,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="22" customWidth="1"/>
     <col min="8" max="8" width="13" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="22"/>
+    <col min="9" max="9" width="29.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>7</v>
       </c>
@@ -2342,10 +2265,10 @@
         <v>10</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>22</v>
       </c>
@@ -2364,7 +2287,7 @@
       <c r="F2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="28" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="21" t="s">
@@ -2373,9 +2296,9 @@
       <c r="I2" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="30"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>24</v>
       </c>
@@ -2394,7 +2317,7 @@
       <c r="F3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="28" t="s">
         <v>39</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -2403,11 +2326,11 @@
       <c r="I3" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="30" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>24</v>
       </c>
@@ -2426,7 +2349,7 @@
       <c r="F4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H4" s="21" t="s">
@@ -2435,9 +2358,11 @@
       <c r="I4" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J4" s="25"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>24</v>
       </c>
@@ -2456,7 +2381,7 @@
       <c r="F5" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="28" t="s">
         <v>28</v>
       </c>
       <c r="H5" s="21" t="s">
@@ -2465,9 +2390,11 @@
       <c r="I5" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J5" s="25"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
@@ -2486,7 +2413,7 @@
       <c r="F6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="28" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="21" t="s">
@@ -2495,9 +2422,9 @@
       <c r="I6" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>24</v>
       </c>
@@ -2516,7 +2443,7 @@
       <c r="F7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="28" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="21" t="s">
@@ -2525,9 +2452,9 @@
       <c r="I7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="30"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>24</v>
       </c>
@@ -2546,7 +2473,7 @@
       <c r="F8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="28" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="21" t="s">
@@ -2555,9 +2482,9 @@
       <c r="I8" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="25"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>24</v>
       </c>
@@ -2576,7 +2503,7 @@
       <c r="F9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="28" t="s">
         <v>44</v>
       </c>
       <c r="H9" s="21" t="s">
@@ -2585,9 +2512,9 @@
       <c r="I9" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J9" s="25"/>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>24</v>
       </c>
@@ -2606,7 +2533,7 @@
       <c r="F10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="28" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="21" t="s">
@@ -2615,9 +2542,9 @@
       <c r="I10" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>24</v>
       </c>
@@ -2636,7 +2563,7 @@
       <c r="F11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="28" t="s">
         <v>43</v>
       </c>
       <c r="H11" s="21" t="s">
@@ -2645,9 +2572,9 @@
       <c r="I11" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J11" s="25"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -2666,7 +2593,7 @@
       <c r="F12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="28" t="s">
         <v>42</v>
       </c>
       <c r="H12" s="21" t="s">
@@ -2675,9 +2602,9 @@
       <c r="I12" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J12" s="25"/>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>24</v>
       </c>
@@ -2696,7 +2623,7 @@
       <c r="F13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="28" t="s">
         <v>41</v>
       </c>
       <c r="H13" s="21" t="s">
@@ -2705,9 +2632,9 @@
       <c r="I13" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J13" s="25"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>24</v>
       </c>
@@ -2726,7 +2653,7 @@
       <c r="F14" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="28" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="21" t="s">
@@ -2735,9 +2662,9 @@
       <c r="I14" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J14" s="25"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="30"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>24</v>
       </c>
@@ -2756,7 +2683,7 @@
       <c r="F15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="28" t="s">
         <v>30</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -2765,9 +2692,9 @@
       <c r="I15" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J15" s="25"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="30"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>24</v>
       </c>
@@ -2786,7 +2713,7 @@
       <c r="F16" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="28" t="s">
         <v>40</v>
       </c>
       <c r="H16" s="21" t="s">
@@ -2795,9 +2722,9 @@
       <c r="I16" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J16" s="25"/>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="30"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>24</v>
       </c>
@@ -2816,7 +2743,7 @@
       <c r="F17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="28" t="s">
         <v>38</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -2825,9 +2752,9 @@
       <c r="I17" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J17" s="25"/>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="30"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
@@ -2846,7 +2773,7 @@
       <c r="F18" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="28" t="s">
         <v>37</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -2855,9 +2782,9 @@
       <c r="I18" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J18" s="25"/>
-    </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="30"/>
+    </row>
+    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>24</v>
       </c>
@@ -2876,7 +2803,7 @@
       <c r="F19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="28" t="s">
         <v>36</v>
       </c>
       <c r="H19" s="21" t="s">
@@ -2885,9 +2812,9 @@
       <c r="I19" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J19" s="25"/>
-    </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>24</v>
       </c>
@@ -2906,7 +2833,7 @@
       <c r="F20" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="28" t="s">
         <v>35</v>
       </c>
       <c r="H20" s="21" t="s">
@@ -2915,9 +2842,9 @@
       <c r="I20" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J20" s="25"/>
-    </row>
-    <row r="21" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="30"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>24</v>
       </c>
@@ -2936,7 +2863,7 @@
       <c r="F21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="28" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="21" t="s">
@@ -2945,11 +2872,11 @@
       <c r="I21" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J21" s="25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>24</v>
       </c>
@@ -2968,7 +2895,7 @@
       <c r="F22" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="28" t="s">
         <v>33</v>
       </c>
       <c r="H22" s="21" t="s">
@@ -2977,9 +2904,9 @@
       <c r="I22" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J22" s="25"/>
-    </row>
-    <row r="23" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="30"/>
+    </row>
+    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>101</v>
       </c>
@@ -2998,7 +2925,7 @@
       <c r="F23" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="28" t="s">
         <v>104</v>
       </c>
       <c r="H23" s="21" t="s">
@@ -3007,11 +2934,11 @@
       <c r="I23" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J23" s="30" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>101</v>
       </c>
@@ -3030,7 +2957,7 @@
       <c r="F24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="28" t="s">
         <v>106</v>
       </c>
       <c r="H24" s="21" t="s">
@@ -3039,9 +2966,9 @@
       <c r="I24" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J24" s="25"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="30"/>
+    </row>
+    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>101</v>
       </c>
@@ -3060,7 +2987,7 @@
       <c r="F25" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="28" t="s">
         <v>105</v>
       </c>
       <c r="H25" s="21" t="s">
@@ -3069,9 +2996,9 @@
       <c r="I25" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J25" s="25"/>
-    </row>
-    <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="30"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>101</v>
       </c>
@@ -3090,7 +3017,7 @@
       <c r="F26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="28" t="s">
         <v>103</v>
       </c>
       <c r="H26" s="21" t="s">
@@ -3099,9 +3026,9 @@
       <c r="I26" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J26" s="25"/>
-    </row>
-    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>101</v>
       </c>
@@ -3120,7 +3047,7 @@
       <c r="F27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="28" t="s">
         <v>102</v>
       </c>
       <c r="H27" s="21" t="s">
@@ -3129,9 +3056,9 @@
       <c r="I27" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J27" s="25"/>
-    </row>
-    <row r="28" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>48</v>
       </c>
@@ -3150,7 +3077,7 @@
       <c r="F28" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="28" t="s">
         <v>76</v>
       </c>
       <c r="H28" s="21" t="s">
@@ -3159,11 +3086,11 @@
       <c r="I28" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="J28" s="30" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>48</v>
       </c>
@@ -3182,7 +3109,7 @@
       <c r="F29" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="28" t="s">
         <v>69</v>
       </c>
       <c r="H29" s="21" t="s">
@@ -3191,11 +3118,11 @@
       <c r="I29" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J29" s="25" t="s">
+      <c r="J29" s="30" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>48</v>
       </c>
@@ -3214,7 +3141,7 @@
       <c r="F30" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="28" t="s">
         <v>66</v>
       </c>
       <c r="H30" s="21" t="s">
@@ -3223,11 +3150,11 @@
       <c r="I30" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J30" s="25" t="s">
+      <c r="J30" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>48</v>
       </c>
@@ -3246,7 +3173,7 @@
       <c r="F31" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G31" s="21" t="s">
+      <c r="G31" s="28" t="s">
         <v>74</v>
       </c>
       <c r="H31" s="21" t="s">
@@ -3255,11 +3182,11 @@
       <c r="I31" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J31" s="25" t="s">
+      <c r="J31" s="30" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>48</v>
       </c>
@@ -3278,7 +3205,7 @@
       <c r="F32" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="28" t="s">
         <v>64</v>
       </c>
       <c r="H32" s="21" t="s">
@@ -3287,11 +3214,11 @@
       <c r="I32" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J32" s="25" t="s">
+      <c r="J32" s="30" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>48</v>
       </c>
@@ -3310,7 +3237,7 @@
       <c r="F33" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="28" t="s">
         <v>59</v>
       </c>
       <c r="H33" s="21" t="s">
@@ -3319,11 +3246,11 @@
       <c r="I33" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J33" s="25" t="s">
+      <c r="J33" s="30" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>48</v>
       </c>
@@ -3342,7 +3269,7 @@
       <c r="F34" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="28" t="s">
         <v>67</v>
       </c>
       <c r="H34" s="21" t="s">
@@ -3351,11 +3278,11 @@
       <c r="I34" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J34" s="25" t="s">
+      <c r="J34" s="30" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>48</v>
       </c>
@@ -3374,7 +3301,7 @@
       <c r="F35" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="28" t="s">
         <v>114</v>
       </c>
       <c r="H35" s="21" t="s">
@@ -3383,11 +3310,11 @@
       <c r="I35" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J35" s="25" t="s">
+      <c r="J35" s="30" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>48</v>
       </c>
@@ -3406,7 +3333,7 @@
       <c r="F36" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="28" t="s">
         <v>49</v>
       </c>
       <c r="H36" s="21" t="s">
@@ -3415,11 +3342,11 @@
       <c r="I36" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J36" s="25" t="s">
+      <c r="J36" s="30" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>48</v>
       </c>
@@ -3438,7 +3365,7 @@
       <c r="F37" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="28" t="s">
         <v>84</v>
       </c>
       <c r="H37" s="21" t="s">
@@ -3447,9 +3374,9 @@
       <c r="I37" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J37" s="25"/>
-    </row>
-    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J37" s="30"/>
+    </row>
+    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>48</v>
       </c>
@@ -3468,7 +3395,7 @@
       <c r="F38" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="28" t="s">
         <v>83</v>
       </c>
       <c r="H38" s="21" t="s">
@@ -3477,9 +3404,9 @@
       <c r="I38" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J38" s="25"/>
-    </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J38" s="30"/>
+    </row>
+    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>48</v>
       </c>
@@ -3498,7 +3425,7 @@
       <c r="F39" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G39" s="28" t="s">
         <v>82</v>
       </c>
       <c r="H39" s="21" t="s">
@@ -3507,9 +3434,9 @@
       <c r="I39" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J39" s="25"/>
-    </row>
-    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="30"/>
+    </row>
+    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>48</v>
       </c>
@@ -3528,7 +3455,7 @@
       <c r="F40" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="28" t="s">
         <v>81</v>
       </c>
       <c r="H40" s="21" t="s">
@@ -3537,9 +3464,11 @@
       <c r="I40" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J40" s="25"/>
-    </row>
-    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J40" s="30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>48</v>
       </c>
@@ -3558,7 +3487,7 @@
       <c r="F41" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="28" t="s">
         <v>80</v>
       </c>
       <c r="H41" s="21" t="s">
@@ -3567,9 +3496,9 @@
       <c r="I41" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J41" s="25"/>
-    </row>
-    <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J41" s="30"/>
+    </row>
+    <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>48</v>
       </c>
@@ -3588,7 +3517,7 @@
       <c r="F42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="28" t="s">
         <v>79</v>
       </c>
       <c r="H42" s="21" t="s">
@@ -3597,9 +3526,9 @@
       <c r="I42" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J42" s="25"/>
-    </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="30"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>48</v>
       </c>
@@ -3618,7 +3547,7 @@
       <c r="F43" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="28" t="s">
         <v>78</v>
       </c>
       <c r="H43" s="21" t="s">
@@ -3627,9 +3556,9 @@
       <c r="I43" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J43" s="25"/>
-    </row>
-    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J43" s="30"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>48</v>
       </c>
@@ -3648,7 +3577,7 @@
       <c r="F44" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="21" t="s">
+      <c r="G44" s="28" t="s">
         <v>77</v>
       </c>
       <c r="H44" s="21" t="s">
@@ -3657,9 +3586,9 @@
       <c r="I44" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J44" s="25"/>
-    </row>
-    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J44" s="30"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>48</v>
       </c>
@@ -3678,7 +3607,7 @@
       <c r="F45" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G45" s="21" t="s">
+      <c r="G45" s="28" t="s">
         <v>75</v>
       </c>
       <c r="H45" s="21" t="s">
@@ -3687,9 +3616,9 @@
       <c r="I45" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J45" s="25"/>
-    </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J45" s="30"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>48</v>
       </c>
@@ -3708,7 +3637,7 @@
       <c r="F46" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="28" t="s">
         <v>73</v>
       </c>
       <c r="H46" s="21" t="s">
@@ -3717,9 +3646,9 @@
       <c r="I46" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J46" s="25"/>
-    </row>
-    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="30"/>
+    </row>
+    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>48</v>
       </c>
@@ -3738,7 +3667,7 @@
       <c r="F47" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="G47" s="28" t="s">
         <v>72</v>
       </c>
       <c r="H47" s="21" t="s">
@@ -3747,9 +3676,9 @@
       <c r="I47" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J47" s="25"/>
-    </row>
-    <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J47" s="30"/>
+    </row>
+    <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>48</v>
       </c>
@@ -3768,7 +3697,7 @@
       <c r="F48" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="28" t="s">
         <v>71</v>
       </c>
       <c r="H48" s="21" t="s">
@@ -3777,9 +3706,9 @@
       <c r="I48" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J48" s="25"/>
-    </row>
-    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J48" s="30"/>
+    </row>
+    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>48</v>
       </c>
@@ -3798,7 +3727,7 @@
       <c r="F49" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="G49" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H49" s="21" t="s">
@@ -3807,9 +3736,9 @@
       <c r="I49" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J49" s="25"/>
-    </row>
-    <row r="50" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J49" s="30"/>
+    </row>
+    <row r="50" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>48</v>
       </c>
@@ -3828,7 +3757,7 @@
       <c r="F50" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="G50" s="28" t="s">
         <v>68</v>
       </c>
       <c r="H50" s="21" t="s">
@@ -3837,9 +3766,9 @@
       <c r="I50" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J50" s="25"/>
-    </row>
-    <row r="51" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J50" s="30"/>
+    </row>
+    <row r="51" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>48</v>
       </c>
@@ -3858,7 +3787,7 @@
       <c r="F51" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="28" t="s">
         <v>65</v>
       </c>
       <c r="H51" s="21" t="s">
@@ -3867,9 +3796,9 @@
       <c r="I51" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J51" s="25"/>
-    </row>
-    <row r="52" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J51" s="30"/>
+    </row>
+    <row r="52" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>48</v>
       </c>
@@ -3888,7 +3817,7 @@
       <c r="F52" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="G52" s="28" t="s">
         <v>63</v>
       </c>
       <c r="H52" s="21" t="s">
@@ -3897,9 +3826,9 @@
       <c r="I52" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J52" s="25"/>
-    </row>
-    <row r="53" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J52" s="30"/>
+    </row>
+    <row r="53" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>48</v>
       </c>
@@ -3918,7 +3847,7 @@
       <c r="F53" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="G53" s="28" t="s">
         <v>62</v>
       </c>
       <c r="H53" s="21" t="s">
@@ -3927,9 +3856,9 @@
       <c r="I53" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J53" s="25"/>
-    </row>
-    <row r="54" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J53" s="30"/>
+    </row>
+    <row r="54" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>48</v>
       </c>
@@ -3948,7 +3877,7 @@
       <c r="F54" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="G54" s="28" t="s">
         <v>61</v>
       </c>
       <c r="H54" s="21" t="s">
@@ -3957,9 +3886,9 @@
       <c r="I54" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J54" s="25"/>
-    </row>
-    <row r="55" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J54" s="30"/>
+    </row>
+    <row r="55" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
         <v>48</v>
       </c>
@@ -3978,7 +3907,7 @@
       <c r="F55" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G55" s="21" t="s">
+      <c r="G55" s="28" t="s">
         <v>60</v>
       </c>
       <c r="H55" s="21" t="s">
@@ -3987,9 +3916,9 @@
       <c r="I55" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J55" s="25"/>
-    </row>
-    <row r="56" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J55" s="30"/>
+    </row>
+    <row r="56" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>48</v>
       </c>
@@ -4008,7 +3937,7 @@
       <c r="F56" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G56" s="21" t="s">
+      <c r="G56" s="28" t="s">
         <v>58</v>
       </c>
       <c r="H56" s="21" t="s">
@@ -4017,9 +3946,9 @@
       <c r="I56" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J56" s="25"/>
-    </row>
-    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J56" s="30"/>
+    </row>
+    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>48</v>
       </c>
@@ -4038,7 +3967,7 @@
       <c r="F57" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G57" s="21" t="s">
+      <c r="G57" s="28" t="s">
         <v>57</v>
       </c>
       <c r="H57" s="21" t="s">
@@ -4047,9 +3976,9 @@
       <c r="I57" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J57" s="25"/>
-    </row>
-    <row r="58" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J57" s="30"/>
+    </row>
+    <row r="58" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>48</v>
       </c>
@@ -4068,7 +3997,7 @@
       <c r="F58" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G58" s="28" t="s">
         <v>56</v>
       </c>
       <c r="H58" s="21" t="s">
@@ -4077,9 +4006,9 @@
       <c r="I58" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J58" s="25"/>
-    </row>
-    <row r="59" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J58" s="30"/>
+    </row>
+    <row r="59" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>48</v>
       </c>
@@ -4098,7 +4027,7 @@
       <c r="F59" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G59" s="21" t="s">
+      <c r="G59" s="28" t="s">
         <v>55</v>
       </c>
       <c r="H59" s="21" t="s">
@@ -4107,9 +4036,9 @@
       <c r="I59" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J59" s="25"/>
-    </row>
-    <row r="60" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J59" s="30"/>
+    </row>
+    <row r="60" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>48</v>
       </c>
@@ -4128,7 +4057,7 @@
       <c r="F60" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G60" s="21" t="s">
+      <c r="G60" s="28" t="s">
         <v>54</v>
       </c>
       <c r="H60" s="21" t="s">
@@ -4137,9 +4066,9 @@
       <c r="I60" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J60" s="25"/>
-    </row>
-    <row r="61" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J60" s="30"/>
+    </row>
+    <row r="61" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>48</v>
       </c>
@@ -4158,18 +4087,18 @@
       <c r="F61" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G61" s="21" t="s">
+      <c r="G61" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H61" s="28" t="s">
+      <c r="H61" s="26" t="s">
         <v>19</v>
       </c>
       <c r="I61" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J61" s="25"/>
-    </row>
-    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J61" s="30"/>
+    </row>
+    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
         <v>48</v>
       </c>
@@ -4188,7 +4117,7 @@
       <c r="F62" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G62" s="21" t="s">
+      <c r="G62" s="28" t="s">
         <v>52</v>
       </c>
       <c r="H62" s="21" t="s">
@@ -4197,9 +4126,9 @@
       <c r="I62" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J62" s="25"/>
-    </row>
-    <row r="63" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J62" s="30"/>
+    </row>
+    <row r="63" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>48</v>
       </c>
@@ -4218,7 +4147,7 @@
       <c r="F63" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G63" s="28" t="s">
         <v>51</v>
       </c>
       <c r="H63" s="21" t="s">
@@ -4227,9 +4156,9 @@
       <c r="I63" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J63" s="25"/>
-    </row>
-    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J63" s="30"/>
+    </row>
+    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
         <v>48</v>
       </c>
@@ -4248,7 +4177,7 @@
       <c r="F64" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G64" s="21" t="s">
+      <c r="G64" s="28" t="s">
         <v>50</v>
       </c>
       <c r="H64" s="21" t="s">
@@ -4257,14 +4186,14 @@
       <c r="I64" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J64" s="25"/>
-    </row>
-    <row r="65" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J64" s="30"/>
+    </row>
+    <row r="65" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C65" s="21" t="s">
         <v>17</v>
@@ -4278,8 +4207,8 @@
       <c r="F65" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G65" s="21" t="s">
-        <v>160</v>
+      <c r="G65" s="28" t="s">
+        <v>94</v>
       </c>
       <c r="H65" s="21" t="s">
         <v>19</v>
@@ -4287,16 +4216,14 @@
       <c r="I65" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J65" s="25" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J65" s="30"/>
+    </row>
+    <row r="66" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C66" s="21" t="s">
         <v>17</v>
@@ -4310,8 +4237,8 @@
       <c r="F66" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G66" s="21" t="s">
-        <v>162</v>
+      <c r="G66" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="H66" s="21" t="s">
         <v>19</v>
@@ -4319,16 +4246,14 @@
       <c r="I66" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J66" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J66" s="30"/>
+    </row>
+    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C67" s="21" t="s">
         <v>17</v>
@@ -4342,8 +4267,8 @@
       <c r="F67" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G67" s="21" t="s">
-        <v>125</v>
+      <c r="G67" s="28" t="s">
+        <v>92</v>
       </c>
       <c r="H67" s="21" t="s">
         <v>19</v>
@@ -4351,16 +4276,14 @@
       <c r="I67" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J67" s="25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J67" s="30"/>
+    </row>
+    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C68" s="21" t="s">
         <v>17</v>
@@ -4374,8 +4297,8 @@
       <c r="F68" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G68" s="21" t="s">
-        <v>126</v>
+      <c r="G68" s="28" t="s">
+        <v>91</v>
       </c>
       <c r="H68" s="21" t="s">
         <v>19</v>
@@ -4383,16 +4306,14 @@
       <c r="I68" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J68" s="25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J68" s="30"/>
+    </row>
+    <row r="69" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C69" s="21" t="s">
         <v>17</v>
@@ -4406,8 +4327,8 @@
       <c r="F69" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G69" s="21" t="s">
-        <v>127</v>
+      <c r="G69" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="H69" s="21" t="s">
         <v>19</v>
@@ -4415,16 +4336,14 @@
       <c r="I69" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J69" s="25" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J69" s="30"/>
+    </row>
+    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C70" s="21" t="s">
         <v>17</v>
@@ -4438,8 +4357,8 @@
       <c r="F70" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G70" s="21" t="s">
-        <v>127</v>
+      <c r="G70" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="H70" s="21" t="s">
         <v>19</v>
@@ -4447,16 +4366,14 @@
       <c r="I70" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J70" s="25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J70" s="30"/>
+    </row>
+    <row r="71" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C71" s="21" t="s">
         <v>17</v>
@@ -4470,8 +4387,8 @@
       <c r="F71" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G71" s="21" t="s">
-        <v>127</v>
+      <c r="G71" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="H71" s="21" t="s">
         <v>19</v>
@@ -4479,16 +4396,14 @@
       <c r="I71" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J71" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J71" s="30"/>
+    </row>
+    <row r="72" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C72" s="21" t="s">
         <v>17</v>
@@ -4502,8 +4417,8 @@
       <c r="F72" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G72" s="21" t="s">
-        <v>151</v>
+      <c r="G72" s="28" t="s">
+        <v>87</v>
       </c>
       <c r="H72" s="21" t="s">
         <v>19</v>
@@ -4511,16 +4426,14 @@
       <c r="I72" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J72" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J72" s="30"/>
+    </row>
+    <row r="73" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C73" s="21" t="s">
         <v>17</v>
@@ -4534,8 +4447,8 @@
       <c r="F73" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G73" s="21" t="s">
-        <v>134</v>
+      <c r="G73" s="28" t="s">
+        <v>97</v>
       </c>
       <c r="H73" s="21" t="s">
         <v>19</v>
@@ -4543,16 +4456,14 @@
       <c r="I73" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J73" s="25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J73" s="30"/>
+    </row>
+    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C74" s="21" t="s">
         <v>17</v>
@@ -4566,8 +4477,8 @@
       <c r="F74" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G74" s="21" t="s">
-        <v>136</v>
+      <c r="G74" s="28" t="s">
+        <v>98</v>
       </c>
       <c r="H74" s="21" t="s">
         <v>19</v>
@@ -4575,639 +4486,46 @@
       <c r="I74" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="J74" s="25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="C75" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E75" s="21">
-        <v>1</v>
-      </c>
-      <c r="F75" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G75" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="H75" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I75" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J75" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B76" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="C76" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E76" s="21">
-        <v>1</v>
-      </c>
-      <c r="F76" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G76" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="H76" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I76" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J76" s="25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B77" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" s="21">
-        <v>1</v>
-      </c>
-      <c r="F77" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G77" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="H77" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I77" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J77" s="25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B78" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E78" s="21">
-        <v>1</v>
-      </c>
-      <c r="F78" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G78" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="H78" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I78" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J78" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B79" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C79" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" s="21">
-        <v>1</v>
-      </c>
-      <c r="F79" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G79" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H79" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I79" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J79" s="25" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B80" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C80" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" s="21">
-        <v>1</v>
-      </c>
-      <c r="F80" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G80" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="H80" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I80" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J80" s="25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B81" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C81" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D81" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E81" s="21">
-        <v>1</v>
-      </c>
-      <c r="F81" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G81" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="H81" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I81" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J81" s="25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B82" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C82" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E82" s="21">
-        <v>1</v>
-      </c>
-      <c r="F82" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G82" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="H82" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I82" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J82" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B83" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C83" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D83" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E83" s="21">
-        <v>1</v>
-      </c>
-      <c r="F83" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G83" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="H83" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I83" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J83" s="25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B84" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C84" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E84" s="21">
-        <v>1</v>
-      </c>
-      <c r="F84" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G84" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="H84" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I84" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J84" s="25"/>
-    </row>
-    <row r="85" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B85" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E85" s="21">
-        <v>1</v>
-      </c>
-      <c r="F85" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G85" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H85" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I85" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J85" s="25"/>
-    </row>
-    <row r="86" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B86" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C86" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D86" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E86" s="21">
-        <v>1</v>
-      </c>
-      <c r="F86" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G86" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="H86" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I86" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J86" s="25"/>
-    </row>
-    <row r="87" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B87" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C87" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E87" s="21">
-        <v>1</v>
-      </c>
-      <c r="F87" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G87" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="H87" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I87" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J87" s="25"/>
-    </row>
-    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C88" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E88" s="21">
-        <v>1</v>
-      </c>
-      <c r="F88" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G88" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="H88" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I88" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J88" s="25"/>
-    </row>
-    <row r="89" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B89" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C89" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E89" s="21">
-        <v>1</v>
-      </c>
-      <c r="F89" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G89" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="H89" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I89" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J89" s="25"/>
-    </row>
-    <row r="90" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B90" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C90" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E90" s="21">
-        <v>1</v>
-      </c>
-      <c r="F90" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G90" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="H90" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I90" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J90" s="25"/>
-    </row>
-    <row r="91" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B91" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C91" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E91" s="21">
-        <v>1</v>
-      </c>
-      <c r="F91" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G91" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="H91" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I91" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J91" s="25"/>
-    </row>
-    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="21" t="s">
+      <c r="J74" s="30"/>
+    </row>
+    <row r="75" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B92" s="21" t="s">
+      <c r="B75" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C92" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D92" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E92" s="21">
-        <v>1</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G92" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="H92" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I92" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J92" s="25"/>
-    </row>
-    <row r="93" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B93" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C93" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D93" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E93" s="21">
-        <v>1</v>
-      </c>
-      <c r="F93" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G93" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="H93" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="I93" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J93" s="25"/>
-    </row>
-    <row r="94" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B94" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C94" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D94" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E94" s="26">
-        <v>1</v>
-      </c>
-      <c r="F94" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G94" s="26" t="s">
+      <c r="C75" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" s="25">
+        <v>1</v>
+      </c>
+      <c r="F75" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G75" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="H94" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I94" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="J94" s="27"/>
+      <c r="H75" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I75" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J75" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J94">
-    <filterColumn colId="9">
-      <filters blank="1"/>
-    </filterColumn>
-    <sortState ref="A2:J94">
-      <sortCondition ref="A2:A94"/>
+  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <sortState ref="A2:J75">
+      <sortCondition ref="A2:A75"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:J94">
-    <sortCondition ref="J2:J94"/>
+  <sortState ref="A2:J75">
+    <sortCondition ref="J2:J75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="22" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
628805: TASK: Requirements Traceability Matrix for IOC Entry TASCore Build 3 in Requirement Folder - Uploaded the RTM for Release 1 after removing the Defect ID's per Release Agent
</commit_message>
<xml_diff>
--- a/TASCore_documents/Requirement/Build 3/TAS_Core_RTM_TAS.01.00.203_20180607_163807.xlsx
+++ b/TASCore_documents/Requirement/Build 3/TAS_Core_RTM_TAS.01.00.203_20180607_163807.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.ballerstein\Desktop\latest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\TASCore Release B3\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042B6D99-D8AB-4BDF-8FE7-A2D0800384F7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17340" windowHeight="4845" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="116">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -350,40 +349,7 @@
     <t>TC2167</t>
   </si>
   <si>
-    <t>DE458</t>
-  </si>
-  <si>
-    <t>DE485</t>
-  </si>
-  <si>
-    <t>DE522</t>
-  </si>
-  <si>
-    <t>DE517</t>
-  </si>
-  <si>
-    <t>DE514</t>
-  </si>
-  <si>
-    <t>DE512</t>
-  </si>
-  <si>
-    <t>DE521</t>
-  </si>
-  <si>
     <t>TC2360</t>
-  </si>
-  <si>
-    <t>DE518</t>
-  </si>
-  <si>
-    <t>DE511</t>
-  </si>
-  <si>
-    <t>DE513</t>
-  </si>
-  <si>
-    <t>DE510</t>
   </si>
   <si>
     <t>TAS.01.00.203_20180607_163807</t>
@@ -434,9 +400,6 @@
     <t>June 18, 2018</t>
   </si>
   <si>
-    <t>DE482</t>
-  </si>
-  <si>
     <t>Final</t>
   </si>
   <si>
@@ -457,17 +420,11 @@
       <t xml:space="preserve">          </t>
     </r>
   </si>
-  <si>
-    <t>was impacted by DE485 (discovered in TC2177)</t>
-  </si>
-  <si>
-    <t>was impacted by DE518 (discovered in TC2362)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1314,7 +1271,7 @@
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
@@ -1592,12 +1549,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Revision_History" displayName="Revision_History" ref="A3:D6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Revision_History" displayName="Revision_History" ref="A3:D6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Version" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Author" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" name="Version" dataDxfId="2"/>
+    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" name="Author" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1923,7 +1880,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1954,7 +1911,7 @@
     </row>
     <row r="6" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2002,7 +1959,7 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
@@ -2014,7 +1971,7 @@
     </row>
     <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
@@ -2071,7 +2028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2128,7 +2085,7 @@
     </row>
     <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B5" s="18">
         <v>2</v>
@@ -2137,21 +2094,21 @@
         <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B6" s="18">
         <v>3</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2209,16 +2166,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2222,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2294,7 +2251,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J2" s="30"/>
     </row>
@@ -2324,11 +2281,9 @@
         <v>19</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>108</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -2356,11 +2311,9 @@
         <v>19</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>128</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J4" s="30"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
@@ -2388,11 +2341,9 @@
         <v>19</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>128</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -2420,7 +2371,7 @@
         <v>19</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J6" s="30"/>
     </row>
@@ -2450,7 +2401,7 @@
         <v>19</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J7" s="30"/>
     </row>
@@ -2480,7 +2431,7 @@
         <v>19</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J8" s="30"/>
     </row>
@@ -2510,7 +2461,7 @@
         <v>19</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J9" s="30"/>
     </row>
@@ -2540,7 +2491,7 @@
         <v>19</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J10" s="30"/>
     </row>
@@ -2570,7 +2521,7 @@
         <v>19</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J11" s="30"/>
     </row>
@@ -2600,7 +2551,7 @@
         <v>19</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J12" s="30"/>
     </row>
@@ -2630,7 +2581,7 @@
         <v>19</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J13" s="30"/>
     </row>
@@ -2660,7 +2611,7 @@
         <v>19</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J14" s="30"/>
     </row>
@@ -2690,7 +2641,7 @@
         <v>19</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J15" s="30"/>
     </row>
@@ -2720,7 +2671,7 @@
         <v>19</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J16" s="30"/>
     </row>
@@ -2750,7 +2701,7 @@
         <v>19</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J17" s="30"/>
     </row>
@@ -2780,7 +2731,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J18" s="30"/>
     </row>
@@ -2810,7 +2761,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J19" s="30"/>
     </row>
@@ -2840,7 +2791,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J20" s="30"/>
     </row>
@@ -2870,11 +2821,9 @@
         <v>19</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>124</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
@@ -2902,7 +2851,7 @@
         <v>19</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J22" s="30"/>
     </row>
@@ -2932,11 +2881,9 @@
         <v>19</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>107</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
@@ -2964,7 +2911,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J24" s="30"/>
     </row>
@@ -2994,7 +2941,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J25" s="30"/>
     </row>
@@ -3024,7 +2971,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J26" s="30"/>
     </row>
@@ -3054,7 +3001,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J27" s="30"/>
     </row>
@@ -3084,11 +3031,9 @@
         <v>19</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J28" s="30" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
@@ -3116,11 +3061,9 @@
         <v>19</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J29" s="30" t="s">
-        <v>116</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
@@ -3148,11 +3091,9 @@
         <v>19</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J30" s="30" t="s">
-        <v>112</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
@@ -3180,11 +3121,9 @@
         <v>19</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J31" s="30" t="s">
-        <v>117</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
@@ -3212,11 +3151,9 @@
         <v>19</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J32" s="30" t="s">
-        <v>111</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J32" s="30"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
@@ -3244,11 +3181,9 @@
         <v>19</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J33" s="30" t="s">
-        <v>110</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J33" s="30"/>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
@@ -3276,11 +3211,9 @@
         <v>19</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>115</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J34" s="30"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
@@ -3302,17 +3235,15 @@
         <v>18</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H35" s="21" t="s">
         <v>19</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J35" s="30" t="s">
-        <v>113</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J35" s="30"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
@@ -3340,11 +3271,9 @@
         <v>19</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J36" s="30" t="s">
-        <v>109</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J36" s="30"/>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
@@ -3372,7 +3301,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J37" s="30"/>
     </row>
@@ -3402,7 +3331,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J38" s="30"/>
     </row>
@@ -3432,7 +3361,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J39" s="30"/>
     </row>
@@ -3462,11 +3391,9 @@
         <v>19</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="J40" s="30" t="s">
-        <v>129</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="J40" s="30"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
@@ -3494,7 +3421,7 @@
         <v>19</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J41" s="30"/>
     </row>
@@ -3524,7 +3451,7 @@
         <v>19</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J42" s="30"/>
     </row>
@@ -3554,7 +3481,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J43" s="30"/>
     </row>
@@ -3584,7 +3511,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J44" s="30"/>
     </row>
@@ -3614,7 +3541,7 @@
         <v>19</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J45" s="30"/>
     </row>
@@ -3644,7 +3571,7 @@
         <v>19</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J46" s="30"/>
     </row>
@@ -3674,7 +3601,7 @@
         <v>19</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J47" s="30"/>
     </row>
@@ -3704,7 +3631,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J48" s="30"/>
     </row>
@@ -3734,7 +3661,7 @@
         <v>19</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J49" s="30"/>
     </row>
@@ -3764,7 +3691,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J50" s="30"/>
     </row>
@@ -3794,7 +3721,7 @@
         <v>19</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J51" s="30"/>
     </row>
@@ -3824,7 +3751,7 @@
         <v>19</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J52" s="30"/>
     </row>
@@ -3854,7 +3781,7 @@
         <v>19</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J53" s="30"/>
     </row>
@@ -3884,7 +3811,7 @@
         <v>19</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J54" s="30"/>
     </row>
@@ -3914,7 +3841,7 @@
         <v>19</v>
       </c>
       <c r="I55" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J55" s="30"/>
     </row>
@@ -3944,7 +3871,7 @@
         <v>19</v>
       </c>
       <c r="I56" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J56" s="30"/>
     </row>
@@ -3974,7 +3901,7 @@
         <v>19</v>
       </c>
       <c r="I57" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J57" s="30"/>
     </row>
@@ -4004,7 +3931,7 @@
         <v>19</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J58" s="30"/>
     </row>
@@ -4034,7 +3961,7 @@
         <v>19</v>
       </c>
       <c r="I59" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J59" s="30"/>
     </row>
@@ -4064,7 +3991,7 @@
         <v>19</v>
       </c>
       <c r="I60" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J60" s="30"/>
     </row>
@@ -4094,7 +4021,7 @@
         <v>19</v>
       </c>
       <c r="I61" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J61" s="30"/>
     </row>
@@ -4124,7 +4051,7 @@
         <v>19</v>
       </c>
       <c r="I62" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J62" s="30"/>
     </row>
@@ -4154,7 +4081,7 @@
         <v>19</v>
       </c>
       <c r="I63" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J63" s="30"/>
     </row>
@@ -4184,7 +4111,7 @@
         <v>19</v>
       </c>
       <c r="I64" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J64" s="30"/>
     </row>
@@ -4214,7 +4141,7 @@
         <v>19</v>
       </c>
       <c r="I65" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J65" s="30"/>
     </row>
@@ -4244,7 +4171,7 @@
         <v>19</v>
       </c>
       <c r="I66" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J66" s="30"/>
     </row>
@@ -4274,7 +4201,7 @@
         <v>19</v>
       </c>
       <c r="I67" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J67" s="30"/>
     </row>
@@ -4304,7 +4231,7 @@
         <v>19</v>
       </c>
       <c r="I68" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J68" s="30"/>
     </row>
@@ -4334,7 +4261,7 @@
         <v>19</v>
       </c>
       <c r="I69" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J69" s="30"/>
     </row>
@@ -4364,7 +4291,7 @@
         <v>19</v>
       </c>
       <c r="I70" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J70" s="30"/>
     </row>
@@ -4394,7 +4321,7 @@
         <v>19</v>
       </c>
       <c r="I71" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J71" s="30"/>
     </row>
@@ -4424,7 +4351,7 @@
         <v>19</v>
       </c>
       <c r="I72" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J72" s="30"/>
     </row>
@@ -4454,7 +4381,7 @@
         <v>19</v>
       </c>
       <c r="I73" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J73" s="30"/>
     </row>
@@ -4484,7 +4411,7 @@
         <v>19</v>
       </c>
       <c r="I74" s="21" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J74" s="30"/>
     </row>
@@ -4514,12 +4441,12 @@
         <v>19</v>
       </c>
       <c r="I75" s="25" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J75" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J75" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A1:J75">
     <sortState ref="A2:J75">
       <sortCondition ref="A2:A75"/>
     </sortState>

</xml_diff>